<commit_message>
Valor imóvel e valor m2
</commit_message>
<xml_diff>
--- a/Apartamentos.xlsx
+++ b/Apartamentos.xlsx
@@ -1,67 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\Busca google maps\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B481ADB-6FE7-4F99-8E95-D3F5D4D34069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4620" yWindow="3690" windowWidth="16440" windowHeight="9810" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Apartamentos" sheetId="1" r:id="rId1"/>
+    <sheet name="Apartamentos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Endereço</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>Valor m²</t>
-  </si>
-  <si>
-    <t>Área</t>
-  </si>
-  <si>
-    <t>Quartos</t>
-  </si>
-  <si>
-    <t>Suites</t>
-  </si>
-  <si>
-    <t>Garagem</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,26 +52,92 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -415,55 +457,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="63.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="37.140625" customWidth="1"/>
+    <col width="63.28515625" customWidth="1" min="2" max="2"/>
+    <col width="21.140625" customWidth="1" style="4" min="3" max="3"/>
+    <col width="15" customWidth="1" style="5" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14.7109375" customWidth="1" min="6" max="6"/>
+    <col width="15.85546875" customWidth="1" min="7" max="7"/>
+    <col width="17.42578125" customWidth="1" min="8" max="8"/>
+    <col width="37.140625" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Endereço</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Valor m²</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Área</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Quartos</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Suites</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Garagem</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="6" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SQN 215, ASA NORTE, BRASILIA</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>5.187</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5.187</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
falta só o link
</commit_message>
<xml_diff>
--- a/Apartamentos.xlsx
+++ b/Apartamentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\Busca google maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F27EE3-12C4-4F50-B7FA-89B1516F03AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66546A7-8077-4F94-946C-494545E14177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2535" yWindow="1860" windowWidth="16440" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Endereço</t>
   </si>
@@ -44,6 +44,24 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>CLNW 2/3, NOROESTE, BRASILIA</t>
+  </si>
+  <si>
+    <t>R$ 4.300</t>
+  </si>
+  <si>
+    <t>R$ 81</t>
+  </si>
+  <si>
+    <t>53 m²</t>
+  </si>
+  <si>
+    <t>2 Quartos</t>
+  </si>
+  <si>
+    <t>1 Vaga</t>
   </si>
 </sst>
 </file>
@@ -481,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -491,11 +509,11 @@
     <col min="2" max="2" width="63.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="15" style="5" customWidth="1"/>
-    <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="37.140625" customWidth="1"/>
+    <col min="5" max="5" width="14" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="37.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -517,17 +535,35 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="C3" s="6"/>

</xml_diff>